<commit_message>
Implementar exporte de materias
</commit_message>
<xml_diff>
--- a/resources/reporte.xlsx
+++ b/resources/reporte.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\IdeaProjects\Uni\Registro-Estudiantes\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\IdeaProjects\Registro Estudiantes\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05752FE7-AE38-412D-9E3D-B3A7C0C6E081}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,37 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>user</author>
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{EC70F134-C36D-491F-A290-C8FBDAB8C072}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>user:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="AC7")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -49,31 +75,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="AC6")</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Usuario:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-jx:each(items="estudiantes" var="estudiante" lastCell="AC6")</t>
+jx:each(items="estudiantes" var="estudiante" lastCell="AC7")</t>
         </r>
       </text>
     </comment>
@@ -82,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>${estudiante.id}</t>
   </si>
@@ -160,13 +162,19 @@
   </si>
   <si>
     <t>Aula: ${seccion.aula}</t>
+  </si>
+  <si>
+    <t>Trimestre:</t>
+  </si>
+  <si>
+    <t>${seccion.trimestre}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +203,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -233,30 +254,21 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
       <right/>
       <top style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -264,31 +276,22 @@
     <border>
       <left/>
       <right style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -297,18 +300,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="1"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -316,10 +319,34 @@
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
@@ -330,28 +357,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -667,265 +703,303 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="28" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="7" width="10.25" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="28" width="3.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="11"/>
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
       <c r="AB2" s="6"/>
-      <c r="AC2" s="13"/>
+      <c r="AC2" s="7"/>
     </row>
     <row r="3" spans="1:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="11"/>
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="10"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="16"/>
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="13"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="16"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4"/>
+      <c r="AC6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B1:Y1"/>
-    <mergeCell ref="B2:Y2"/>
-    <mergeCell ref="D5:H5"/>
+  <mergeCells count="7">
+    <mergeCell ref="B1:AC1"/>
     <mergeCell ref="D6:H6"/>
-    <mergeCell ref="I5:AB5"/>
-    <mergeCell ref="I3:AB3"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I6:AB6"/>
+    <mergeCell ref="I4:AC5"/>
+    <mergeCell ref="B2:AC2"/>
+    <mergeCell ref="B3:AC3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>